<commit_message>
Automatiação da geração de xlsx
</commit_message>
<xml_diff>
--- a/Aldo/estoque.xlsx
+++ b/Aldo/estoque.xlsx
@@ -440,47 +440,47 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>medicamento_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>lote</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>validade</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>custo</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>quant_inicial</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>quant_venda</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>quant_atual</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>medicamento_id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>validade</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>custo</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>quant_inicial</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>quant_venda</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>lote</t>
         </is>
       </c>
     </row>

</xml_diff>